<commit_message>
Writer y Reader partidos
</commit_message>
<xml_diff>
--- a/src/main/resources/data/disponibilidades/disponibilidades_06 23 a 29 2025.xlsx
+++ b/src/main/resources/data/disponibilidades/disponibilidades_06 23 a 29 2025.xlsx
@@ -202,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -210,6 +210,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
@@ -365,8 +371,8 @@
         <v>15</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>

</xml_diff>